<commit_message>
i bins jez feadi
</commit_message>
<xml_diff>
--- a/lu3/opv_messungen.xlsx
+++ b/lu3/opv_messungen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24300" windowHeight="13260" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="aufgabe1" sheetId="1" r:id="rId1"/>
@@ -125,19 +125,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,24 +140,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,6 +157,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,10 +178,26 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -200,8 +208,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,30 +224,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,14 +247,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -275,9 +254,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,7 +298,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,7 +310,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,13 +322,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,43 +352,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,7 +364,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,37 +388,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,19 +400,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +424,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,26 +486,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -556,16 +549,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -595,145 +588,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -747,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -950,7 +943,7 @@
                   <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>800000</c:v>
@@ -1388,103 +1381,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>750000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3006,6 +2999,1595 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"-47x Verst."</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-47x Verst.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>aufgabe2!$A$38:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>aufgabe2!$F$38:$F$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>33.4823237347411</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.9317365937305</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.812413213641</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.4306351197816</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.1603626662683</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.4516783568618</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.2551566336315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.4542688399224</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.2948182990655</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.275010104305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.4796314337637</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.1552028305213</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.9517769134565</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.6587311560206</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.2221624061072</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.7151496021113</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.9559433953591</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.4213572454347</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.3471184205204</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.3194069091384</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.1295441248335</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24.2437520880792</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21.0075951252292</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18.5165514924948</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.9019608002851</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.8813608870055</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.43683213072998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.21179420598498</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.915149811213503</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-3.09803919971486</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"fg1"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fg1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>aufgabe2!$H$37:$H$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>26000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>aufgabe2!$F$37:$F$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.4823237347411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.9317365937305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.812413213641</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.4306351197816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.1603626662683</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.4516783568618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.2551566336315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.4542688399224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.2948182990655</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.275010104305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.4796314337637</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.1552028305213</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.9517769134565</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.6587311560206</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.2221624061072</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.7151496021113</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.9559433953591</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.4213572454347</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.3471184205204</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.3194069091384</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.1295441248335</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.2437520880792</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.0075951252292</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.5165514924948</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.9019608002851</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.8813608870055</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.43683213072998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.21179420598498</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.915149811213503</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.09803919971486</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"-4,7x Verst."</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-4,7x Verst.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>aufgabe2!$A$75:$A$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>650000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="29" c:formatCode="0.00E+00">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>aufgabe2!$F$75:$F$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.2132032617976</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0411998265592</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.0411998265592</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.5023672673787</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.5023672673787</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.5023672673787</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.0037211829031</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.7364419517435</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.0192380205782</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.4747743003499</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.62727528317975</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.85393906519331</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.02794248640903</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.8278537031645</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.526578774446982</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.17189430531695</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.85508106473797</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-3.5636849712305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"fg2"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fg2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>aufgabe2!$H$74:$H$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>230000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>230000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>aufgabe2!$F$37:$F$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.4823237347411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.9317365937305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.812413213641</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.4306351197816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.1603626662683</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.4516783568618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.2551566336315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.4542688399224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.2948182990655</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.275010104305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.4796314337637</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.1552028305213</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.9517769134565</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.6587311560206</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.2221624061072</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.7151496021113</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.9559433953591</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.4213572454347</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.3471184205204</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.3194069091384</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.1295441248335</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.2437520880792</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.0075951252292</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.5165514924948</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.9019608002851</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.8813608870055</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.43683213072998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.21179420598498</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.915149811213503</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.09803919971486</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"ft"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>aufgabe2!$I$37:$I$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>700000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>aufgabe2!$F$37:$F$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.4823237347411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.9317365937305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.812413213641</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.4306351197816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.1603626662683</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.4516783568618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.2551566336315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.4542688399224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.2948182990655</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.275010104305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.4796314337637</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.1552028305213</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.9517769134565</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.6587311560206</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.2221624061072</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.7151496021113</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.9559433953591</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.4213572454347</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.3471184205204</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.3194069091384</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.1295441248335</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.2437520880792</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.0075951252292</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.5165514924948</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.9019608002851</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.8813608870055</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.43683213072998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.21179420598498</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.915149811213503</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.09803919971486</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="367669567"/>
+        <c:axId val="767131436"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="367669567"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr vertOverflow="ellipsis" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" defTabSz="914400">
+                  <a:defRPr sz="1000" kern="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="x-none" altLang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Frequenz [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="x-none" altLang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="767131436"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="767131436"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="40"/>
+          <c:min val="-5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr vertOverflow="ellipsis" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" defTabSz="914400">
+                  <a:defRPr sz="1000" kern="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="x-none" altLang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Amplitude [dB]</a:t>
+                </a:r>
+                <a:endParaRPr lang="x-none" altLang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="367669567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="de-AT" sz="1000" kern="1200">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3047,6 +4629,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4118,6 +5740,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4180,6 +6318,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>387985</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>14605</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>727075</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>109220</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8586470" y="9082405"/>
+        <a:ext cx="6357620" cy="3333115"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4196,8 +6364,8 @@
     </cdr:to>
     <cdr:sp>
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
       </cdr:nvSpPr>
       <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -4235,8 +6403,8 @@
     </cdr:to>
     <cdr:sp>
       <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 2"/>
-        <cdr:cNvSpPr txBox="1"/>
+        <cdr:cNvPr id="3" name="Rectangle 2"/>
+        <cdr:cNvSpPr/>
       </cdr:nvSpPr>
       <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -4279,8 +6447,8 @@
     </cdr:to>
     <cdr:sp>
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
       </cdr:nvSpPr>
       <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -4318,8 +6486,8 @@
     </cdr:to>
     <cdr:sp>
       <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 2"/>
-        <cdr:cNvSpPr txBox="1"/>
+        <cdr:cNvPr id="3" name="Rectangle 2"/>
+        <cdr:cNvSpPr/>
       </cdr:nvSpPr>
       <cdr:spPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -5090,10 +7258,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="L102" sqref="L102"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
@@ -5348,7 +7516,7 @@
         <v>26000</v>
       </c>
       <c r="I37" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -5372,7 +7540,7 @@
         <v>26000</v>
       </c>
       <c r="I38" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -5389,14 +7557,14 @@
         <v>180</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="F39:F67" si="0">20*LOG10(C39/B39)</f>
+        <f t="shared" ref="F39:F68" si="0">20*LOG10(C39/B39)</f>
         <v>32.9317365937305</v>
       </c>
       <c r="H39" s="2">
         <v>26000</v>
       </c>
       <c r="I39" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -5420,7 +7588,7 @@
         <v>26000</v>
       </c>
       <c r="I40" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -5444,7 +7612,7 @@
         <v>26000</v>
       </c>
       <c r="I41" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -5468,7 +7636,7 @@
         <v>26000</v>
       </c>
       <c r="I42" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -5492,7 +7660,7 @@
         <v>26000</v>
       </c>
       <c r="I43" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -5516,7 +7684,7 @@
         <v>26000</v>
       </c>
       <c r="I44" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -5540,7 +7708,7 @@
         <v>26000</v>
       </c>
       <c r="I45" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -5564,7 +7732,7 @@
         <v>26000</v>
       </c>
       <c r="I46" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -5588,7 +7756,7 @@
         <v>26000</v>
       </c>
       <c r="I47" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -5612,7 +7780,7 @@
         <v>26000</v>
       </c>
       <c r="I48" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -5636,7 +7804,7 @@
         <v>26000</v>
       </c>
       <c r="I49" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -5660,7 +7828,7 @@
         <v>26000</v>
       </c>
       <c r="I50" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -5684,7 +7852,7 @@
         <v>26000</v>
       </c>
       <c r="I51" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -5708,7 +7876,7 @@
         <v>26000</v>
       </c>
       <c r="I52" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -5732,7 +7900,7 @@
         <v>26000</v>
       </c>
       <c r="I53" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -5756,7 +7924,7 @@
         <v>26000</v>
       </c>
       <c r="I54" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -5780,7 +7948,7 @@
         <v>26000</v>
       </c>
       <c r="I55" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -5804,7 +7972,7 @@
         <v>26000</v>
       </c>
       <c r="I56" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -5828,7 +7996,7 @@
         <v>26000</v>
       </c>
       <c r="I57" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -5852,7 +8020,7 @@
         <v>26000</v>
       </c>
       <c r="I58" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -5876,7 +8044,7 @@
         <v>26000</v>
       </c>
       <c r="I59" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -5900,7 +8068,7 @@
         <v>26000</v>
       </c>
       <c r="I60" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -5924,7 +8092,7 @@
         <v>26000</v>
       </c>
       <c r="I61" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -5948,7 +8116,7 @@
         <v>26000</v>
       </c>
       <c r="I62" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -5972,7 +8140,7 @@
         <v>26000</v>
       </c>
       <c r="I63" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -5996,7 +8164,7 @@
         <v>26000</v>
       </c>
       <c r="I64" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -6020,12 +8188,12 @@
         <v>26000</v>
       </c>
       <c r="I65" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1">
-        <v>750000</v>
+        <v>700000</v>
       </c>
       <c r="B66" s="1">
         <v>0.1</v>
@@ -6034,14 +8202,14 @@
         <v>0.1</v>
       </c>
       <c r="F66">
-        <f>20*LOG10(C66/B66)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H66" s="2">
         <v>26000</v>
       </c>
       <c r="I66" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -6058,14 +8226,14 @@
         <v>62</v>
       </c>
       <c r="F67">
-        <f>20*LOG10(C67/B67)</f>
+        <f t="shared" si="0"/>
         <v>-0.915149811213503</v>
       </c>
       <c r="H67" s="2">
         <v>26000</v>
       </c>
       <c r="I67" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -6082,14 +8250,14 @@
         <v>57</v>
       </c>
       <c r="F68">
-        <f>20*LOG10(C68/B68)</f>
+        <f t="shared" si="0"/>
         <v>-3.09803919971486</v>
       </c>
       <c r="H68" s="2">
         <v>26000</v>
       </c>
       <c r="I68" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="69" spans="6:9">
@@ -6100,7 +8268,7 @@
         <v>26000</v>
       </c>
       <c r="I69" s="2">
-        <v>750000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="71" spans="1:1">
@@ -6675,7 +8843,7 @@
         <v>0.247</v>
       </c>
       <c r="F97">
-        <f>20*LOG10(C97/B97)</f>
+        <f t="shared" si="1"/>
         <v>7.85393906519331</v>
       </c>
       <c r="H97" s="2">
@@ -6699,7 +8867,7 @@
         <v>96</v>
       </c>
       <c r="F98">
-        <f>20*LOG10(C98/B98)</f>
+        <f t="shared" si="1"/>
         <v>4.02794248640903</v>
       </c>
       <c r="H98" s="2">
@@ -6723,7 +8891,7 @@
         <v>82</v>
       </c>
       <c r="F99">
-        <f>20*LOG10(C99/B99)</f>
+        <f t="shared" si="1"/>
         <v>0.8278537031645</v>
       </c>
       <c r="H99" s="2">
@@ -6747,7 +8915,7 @@
         <v>79</v>
       </c>
       <c r="F100">
-        <f>20*LOG10(C100/B100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H100" s="2">
@@ -6771,7 +8939,7 @@
         <v>75</v>
       </c>
       <c r="F101">
-        <f>20*LOG10(C101/B101)</f>
+        <f t="shared" si="1"/>
         <v>-0.526578774446982</v>
       </c>
       <c r="H101" s="2">
@@ -6795,7 +8963,7 @@
         <v>75</v>
       </c>
       <c r="F102">
-        <f>20*LOG10(C102/B102)</f>
+        <f t="shared" si="1"/>
         <v>-1.17189430531695</v>
       </c>
       <c r="H102" s="2">
@@ -6819,7 +8987,7 @@
         <v>73</v>
       </c>
       <c r="F103">
-        <f>20*LOG10(C103/B103)</f>
+        <f t="shared" si="1"/>
         <v>-1.85508106473797</v>
       </c>
       <c r="H103" s="2">
@@ -6843,7 +9011,7 @@
         <v>64</v>
       </c>
       <c r="F104">
-        <f>20*LOG10(C104/B104)</f>
+        <f t="shared" si="1"/>
         <v>-3.5636849712305</v>
       </c>
       <c r="H104" s="2">
@@ -6864,8 +9032,14 @@
         <v>700000</v>
       </c>
     </row>
+    <row r="106" spans="8:8">
+      <c r="H106">
+        <v>230000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>